<commit_message>
Added run example data
Signed-off-by: shsymoen <steffen.symoens@ugent.be>
</commit_message>
<xml_diff>
--- a/Samples Naphtha2.xlsx
+++ b/Samples Naphtha2.xlsx
@@ -5,23 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="NI -0.3" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="NI 2.6" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="NI 7.0" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="NI 8.2" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="NI 9.3" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="NI03" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NI26" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="NI70" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="NI82" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="NI93" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Titles" vbProcedure="false">'NI 9.3'!$1:$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'NI 9.3'!$A$9:$G$82</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="MPRO_GUID_b06082f287a743159417f47d4a575cdd" vbProcedure="false">'NI -0.3'!$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="MPRO_GUID_02fe1bf97c5a4417b851dcc551db051d" vbProcedure="false">'NI 2.6'!$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="MPRO_GUID_da9806cd8226422c9dc353bf3803eefe" vbProcedure="false">'NI 7.0'!$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="MPRO_GUID_ca0d1a456af847698ccff9b208307159" vbProcedure="false">'NI 8.2'!$A$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="MPRO_GUID_8f1f7177378140e384cd8a0659d2bd9f" vbProcedure="false">'NI 9.3'!$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Titles" vbProcedure="false">NI93!$1:$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">NI93!$A$9:$G$82</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="MPRO_GUID_b06082f287a743159417f47d4a575cdd" vbProcedure="false">NI03!$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="MPRO_GUID_02fe1bf97c5a4417b851dcc551db051d" vbProcedure="false">NI26!$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="MPRO_GUID_da9806cd8226422c9dc353bf3803eefe" vbProcedure="false">NI70!$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="MPRO_GUID_ca0d1a456af847698ccff9b208307159" vbProcedure="false">NI82!$A$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="MPRO_GUID_8f1f7177378140e384cd8a0659d2bd9f" vbProcedure="false">NI93!$A$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1407,15 +1407,15 @@
   </sheetPr>
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.29"/>
@@ -2955,7 +2955,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2975,11 +2975,11 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.29"/>
@@ -4414,7 +4414,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4434,11 +4434,11 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.29"/>
@@ -6188,7 +6188,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6208,11 +6208,11 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.29"/>
@@ -7537,7 +7537,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7553,21 +7553,21 @@
   </sheetPr>
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="11.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="15.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="8" style="6" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="8" style="6" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="11.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9255,7 +9255,7 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="100" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;"Arial,Bold"&amp;12m:lab2 Laboratory Monitoring</oddHeader>
-    <oddFooter>&amp;L&amp;8Printed: &amp;D &amp;T&amp;C&amp;8m:pro-Application: mLab2, User: J0443338&amp;R&amp;8Page &amp;P of &amp;N </oddFooter>
+    <oddFooter>&amp;L&amp;8Printed: &amp;D &amp;T&amp;C&amp;8m:pro-Application: mLab2, User: J0443338&amp;R&amp;8Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>